<commit_message>
Implementação de instruções do simulador
Instruções de deslocamento, condicionais e acesso ao acumulador
</commit_message>
<xml_diff>
--- a/Tabela de Instruções.xlsx
+++ b/Tabela de Instruções.xlsx
@@ -934,7 +934,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -979,8 +979,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -999,6 +1005,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1012,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1128,6 +1140,13 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1410,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2165,7 +2184,7 @@
       <c r="B32" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="47" t="s">
         <v>138</v>
       </c>
       <c r="D32" s="11" t="s">
@@ -2190,7 +2209,7 @@
       <c r="B33" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="51" t="s">
         <v>143</v>
       </c>
       <c r="D33" s="11" t="s">
@@ -2215,7 +2234,7 @@
       <c r="B34" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="47" t="s">
         <v>148</v>
       </c>
       <c r="D34" s="11" t="s">
@@ -2253,7 +2272,7 @@
       <c r="B36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="47" t="s">
         <v>154</v>
       </c>
       <c r="D36" s="11" t="s">
@@ -2278,7 +2297,7 @@
       <c r="B37" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="47" t="s">
         <v>158</v>
       </c>
       <c r="D37" s="11" t="s">
@@ -2303,7 +2322,7 @@
       <c r="B38" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="49" t="s">
         <v>162</v>
       </c>
       <c r="D38" s="11" t="s">
@@ -2382,7 +2401,7 @@
       <c r="B41" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="47" t="s">
         <v>177</v>
       </c>
       <c r="D41" s="11" t="s">
@@ -2522,7 +2541,7 @@
       <c r="B47" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="47" t="s">
         <v>202</v>
       </c>
       <c r="D47" s="11" t="s">
@@ -2547,7 +2566,7 @@
       <c r="B48" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="47" t="s">
         <v>205</v>
       </c>
       <c r="D48" s="11" t="s">
@@ -2568,11 +2587,11 @@
       <c r="I48" s="9"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="52" t="s">
         <v>209</v>
       </c>
       <c r="D49" s="11" t="s">
@@ -2635,7 +2654,7 @@
       <c r="B52" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="49" t="s">
         <v>218</v>
       </c>
       <c r="D52" s="11" t="s">
@@ -2660,7 +2679,7 @@
       <c r="B53" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="47" t="s">
         <v>223</v>
       </c>
       <c r="D53" s="11" t="s">

</xml_diff>

<commit_message>
Marcação das instruções que serão usadas no Problema 2
</commit_message>
<xml_diff>
--- a/Tabela de Instruções.xlsx
+++ b/Tabela de Instruções.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bitnami\PBLSD2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PH\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -986,7 +986,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1001,7 +1001,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1018,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1122,25 +1128,82 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1418,7 +1481,7 @@
   <dimension ref="A1:I1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1466,7 +1529,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="7"/>
@@ -1474,87 +1537,87 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="53"/>
+      <c r="B3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="10" t="s">
+      <c r="I3" s="58"/>
+    </row>
+    <row r="4" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="68"/>
+      <c r="B4" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="10" t="s">
+      <c r="I4" s="58"/>
+    </row>
+    <row r="5" spans="1:9" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="64"/>
+      <c r="B5" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="66"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="49" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -1579,7 +1642,7 @@
       <c r="B7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="50" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="17" t="s">
@@ -1604,7 +1667,7 @@
       <c r="B8" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="50" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="17" t="s">
@@ -1654,7 +1717,7 @@
       <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="11" t="s">
@@ -1679,7 +1742,7 @@
       <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="49" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -1771,7 +1834,7 @@
       <c r="B15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="49" t="s">
         <v>66</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -1796,7 +1859,7 @@
       <c r="B16" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="52" t="s">
         <v>72</v>
       </c>
       <c r="D16" s="11" t="s">
@@ -1821,7 +1884,7 @@
       <c r="B17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="49" t="s">
         <v>76</v>
       </c>
       <c r="D17" s="11" t="s">
@@ -1846,7 +1909,7 @@
       <c r="B18" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="47" t="s">
         <v>82</v>
       </c>
       <c r="D18" s="29" t="s">
@@ -1865,7 +1928,7 @@
       <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="49" t="s">
         <v>84</v>
       </c>
       <c r="D19" s="11" t="s">
@@ -1915,7 +1978,7 @@
       <c r="B21" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="49" t="s">
         <v>94</v>
       </c>
       <c r="D21" s="11" t="s">
@@ -2015,37 +2078,37 @@
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="10" t="s">
+    <row r="26" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="53"/>
+      <c r="B26" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="I26" s="9"/>
+      <c r="I26" s="58"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="49" t="s">
         <v>117</v>
       </c>
       <c r="D27" s="11" t="s">
@@ -2167,37 +2230,37 @@
       </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="10" t="s">
+    <row r="32" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="53"/>
+      <c r="B32" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="57" t="s">
         <v>142</v>
       </c>
-      <c r="I32" s="9"/>
+      <c r="I32" s="58"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="49" t="s">
         <v>143</v>
       </c>
       <c r="D33" s="11" t="s">
@@ -2222,7 +2285,7 @@
       <c r="B34" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="49" t="s">
         <v>148</v>
       </c>
       <c r="D34" s="11" t="s">
@@ -2260,7 +2323,7 @@
       <c r="B36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="49" t="s">
         <v>154</v>
       </c>
       <c r="D36" s="11" t="s">
@@ -2285,7 +2348,7 @@
       <c r="B37" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="47" t="s">
+      <c r="C37" s="49" t="s">
         <v>158</v>
       </c>
       <c r="D37" s="11" t="s">
@@ -2310,7 +2373,7 @@
       <c r="B38" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="52" t="s">
         <v>162</v>
       </c>
       <c r="D38" s="11" t="s">
@@ -2389,7 +2452,7 @@
       <c r="B41" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="47" t="s">
+      <c r="C41" s="49" t="s">
         <v>177</v>
       </c>
       <c r="D41" s="11" t="s">
@@ -2474,62 +2537,62 @@
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="10" t="s">
+    <row r="45" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="53"/>
+      <c r="B45" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="47" t="s">
+      <c r="C45" s="54" t="s">
         <v>191</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="54" t="s">
         <v>192</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="G45" s="13" t="s">
+      <c r="G45" s="56" t="s">
         <v>194</v>
       </c>
-      <c r="H45" s="14" t="s">
+      <c r="H45" s="57" t="s">
         <v>195</v>
       </c>
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="10" t="s">
+      <c r="I45" s="58"/>
+    </row>
+    <row r="46" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="53"/>
+      <c r="B46" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="C46" s="47" t="s">
+      <c r="C46" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D46" s="54" t="s">
         <v>198</v>
       </c>
-      <c r="E46" s="32" t="s">
+      <c r="E46" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="13" t="s">
+      <c r="G46" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="H46" s="14" t="s">
+      <c r="H46" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="I46" s="9"/>
+      <c r="I46" s="58"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C47" s="47" t="s">
+      <c r="C47" s="49" t="s">
         <v>202</v>
       </c>
       <c r="D47" s="11" t="s">
@@ -2554,7 +2617,7 @@
       <c r="B48" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="47" t="s">
+      <c r="C48" s="49" t="s">
         <v>205</v>
       </c>
       <c r="D48" s="11" t="s">
@@ -2575,11 +2638,11 @@
       <c r="I48" s="9"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="51"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="49" t="s">
+      <c r="C49" s="52" t="s">
         <v>209</v>
       </c>
       <c r="D49" s="11" t="s">
@@ -2604,7 +2667,7 @@
       <c r="B50" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="47" t="s">
+      <c r="C50" s="49" t="s">
         <v>213</v>
       </c>
       <c r="D50" s="11" t="s">
@@ -2629,7 +2692,7 @@
         <v>217</v>
       </c>
       <c r="B51" s="7"/>
-      <c r="C51" s="8"/>
+      <c r="C51" s="51"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
       <c r="F51" s="7"/>
@@ -2637,37 +2700,37 @@
       <c r="H51" s="9"/>
       <c r="I51" s="9"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="B52" s="10" t="s">
+    <row r="52" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="53"/>
+      <c r="B52" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="49" t="s">
+      <c r="C52" s="55" t="s">
         <v>218</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="54" t="s">
         <v>219</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E52" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="54" t="s">
         <v>220</v>
       </c>
-      <c r="G52" s="13" t="s">
+      <c r="G52" s="56" t="s">
         <v>221</v>
       </c>
-      <c r="H52" s="14" t="s">
+      <c r="H52" s="57" t="s">
         <v>222</v>
       </c>
-      <c r="I52" s="9"/>
+      <c r="I52" s="58"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="47" t="s">
+      <c r="C53" s="49" t="s">
         <v>223</v>
       </c>
       <c r="D53" s="11" t="s">
@@ -2750,30 +2813,30 @@
       <c r="H56" s="9"/>
       <c r="I56" s="9"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="10" t="s">
+    <row r="57" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="53"/>
+      <c r="B57" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="C57" s="47" t="s">
+      <c r="C57" s="54" t="s">
         <v>239</v>
       </c>
-      <c r="D57" s="32" t="s">
+      <c r="D57" s="54" t="s">
         <v>240</v>
       </c>
-      <c r="E57" s="32" t="s">
+      <c r="E57" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G57" s="36" t="s">
+      <c r="G57" s="56" t="s">
         <v>241</v>
       </c>
-      <c r="H57" s="14" t="s">
+      <c r="H57" s="57" t="s">
         <v>242</v>
       </c>
-      <c r="I57" s="9"/>
+      <c r="I57" s="58"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="27"/>
@@ -2798,30 +2861,30 @@
       </c>
       <c r="I58" s="9"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="10" t="s">
+    <row r="59" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="53"/>
+      <c r="B59" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="47" t="s">
+      <c r="C59" s="54" t="s">
         <v>247</v>
       </c>
-      <c r="D59" s="32" t="s">
+      <c r="D59" s="54" t="s">
         <v>248</v>
       </c>
-      <c r="E59" s="32" t="s">
+      <c r="E59" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F59" s="10" t="s">
+      <c r="F59" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G59" s="36" t="s">
+      <c r="G59" s="56" t="s">
         <v>249</v>
       </c>
-      <c r="H59" s="14" t="s">
+      <c r="H59" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="I59" s="9"/>
+      <c r="I59" s="58"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="27"/>
@@ -2848,80 +2911,80 @@
       </c>
       <c r="I60" s="9"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="10" t="s">
+    <row r="61" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="53"/>
+      <c r="B61" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="C61" s="47" t="s">
+      <c r="C61" s="54" t="s">
         <v>255</v>
       </c>
-      <c r="D61" s="32" t="s">
+      <c r="D61" s="54" t="s">
         <v>256</v>
       </c>
-      <c r="E61" s="32" t="s">
+      <c r="E61" s="54" t="s">
         <v>257</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="F61" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G61" s="36" t="s">
+      <c r="G61" s="56" t="s">
         <v>258</v>
       </c>
-      <c r="H61" s="14" t="s">
+      <c r="H61" s="57" t="s">
         <v>259</v>
       </c>
-      <c r="I61" s="9"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="40"/>
-      <c r="B62" s="16" t="s">
+      <c r="I61" s="58"/>
+    </row>
+    <row r="62" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="60"/>
+      <c r="B62" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="48" t="s">
+      <c r="C62" s="61" t="s">
         <v>260</v>
       </c>
-      <c r="D62" s="41" t="s">
+      <c r="D62" s="61" t="s">
         <v>261</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="F62" s="16" t="s">
+      <c r="F62" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="G62" s="42" t="s">
+      <c r="G62" s="62" t="s">
         <v>262</v>
       </c>
-      <c r="H62" s="20" t="s">
+      <c r="H62" s="63" t="s">
         <v>263</v>
       </c>
-      <c r="I62" s="9"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="10" t="s">
+      <c r="I62" s="58"/>
+    </row>
+    <row r="63" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="53"/>
+      <c r="B63" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="C63" s="47" t="s">
+      <c r="C63" s="54" t="s">
         <v>264</v>
       </c>
-      <c r="D63" s="32" t="s">
+      <c r="D63" s="54" t="s">
         <v>265</v>
       </c>
-      <c r="E63" s="32" t="s">
+      <c r="E63" s="54" t="s">
         <v>257</v>
       </c>
-      <c r="F63" s="10" t="s">
+      <c r="F63" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G63" s="36" t="s">
+      <c r="G63" s="56" t="s">
         <v>266</v>
       </c>
-      <c r="H63" s="14" t="s">
+      <c r="H63" s="57" t="s">
         <v>267</v>
       </c>
-      <c r="I63" s="9"/>
+      <c r="I63" s="58"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="40"/>
@@ -2986,30 +3049,30 @@
       </c>
       <c r="I66" s="9"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="10" t="s">
+    <row r="67" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="53"/>
+      <c r="B67" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="C67" s="47" t="s">
+      <c r="C67" s="54" t="s">
         <v>277</v>
       </c>
-      <c r="D67" s="32" t="s">
+      <c r="D67" s="54" t="s">
         <v>278</v>
       </c>
-      <c r="E67" s="32" t="s">
+      <c r="E67" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F67" s="10" t="s">
+      <c r="F67" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G67" s="36" t="s">
+      <c r="G67" s="56" t="s">
         <v>279</v>
       </c>
-      <c r="H67" s="14" t="s">
+      <c r="H67" s="57" t="s">
         <v>280</v>
       </c>
-      <c r="I67" s="9"/>
+      <c r="I67" s="58"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
@@ -3086,30 +3149,30 @@
       </c>
       <c r="I70" s="9"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="10" t="s">
+    <row r="71" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="53"/>
+      <c r="B71" s="54" t="s">
         <v>206</v>
       </c>
-      <c r="C71" s="47" t="s">
+      <c r="C71" s="54" t="s">
         <v>293</v>
       </c>
-      <c r="D71" s="32" t="s">
+      <c r="D71" s="54" t="s">
         <v>286</v>
       </c>
-      <c r="E71" s="32" t="s">
+      <c r="E71" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F71" s="10" t="s">
+      <c r="F71" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G71" s="43" t="s">
+      <c r="G71" s="56" t="s">
         <v>294</v>
       </c>
-      <c r="H71" s="14" t="s">
+      <c r="H71" s="57" t="s">
         <v>295</v>
       </c>
-      <c r="I71" s="9"/>
+      <c r="I71" s="58"/>
     </row>
     <row r="72" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="44"/>

</xml_diff>